<commit_message>
Committing current files for new repo
</commit_message>
<xml_diff>
--- a/excel_templates/Monthly-Report-Attendance.xlsx
+++ b/excel_templates/Monthly-Report-Attendance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\report_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\scan-admin\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB777F8-8152-4556-B67D-1F32AEC79749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DBAFDA-842C-4AA6-8833-5944BB4D0F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DE17FEAD-50E3-4255-8AE3-87AAD3F49AF3}"/>
   </bookViews>
@@ -782,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110E3B37-164E-4EFB-A183-59C2908E22FD}">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1434,21 +1434,181 @@
       <c r="M39" s="19"/>
       <c r="N39" s="20"/>
     </row>
-    <row r="40" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="26"/>
-      <c r="N40" s="27"/>
+    <row r="40" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="20"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="20"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="20"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="14"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="20"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="14"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="20"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="20"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="14"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="20"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="20"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="20"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="20"/>
+    </row>
+    <row r="50" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="26"/>
+      <c r="N50" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>